<commit_message>
Commit before further improvements
</commit_message>
<xml_diff>
--- a/Additional_Data/Strava_data_dictionary.xlsx
+++ b/Additional_Data/Strava_data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DHB/Documents/My stuff/Strava webscraping/Additional_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F952DBA1-5FEF-B949-9554-714703E36DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD65B4C2-8903-1241-9607-E86394C6C54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1500" windowWidth="24640" windowHeight="13020" xr2:uid="{2E5D1DAE-8741-6A4D-81CE-164A557E1943}"/>
+    <workbookView xWindow="6400" yWindow="500" windowWidth="19200" windowHeight="13000" xr2:uid="{2E5D1DAE-8741-6A4D-81CE-164A557E1943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>Column Name</t>
   </si>
@@ -176,21 +176,41 @@
     <t>Should certainly agree but more values picked up by form. For Rowing, if =0: erg, if not: water</t>
   </si>
   <si>
-    <t>Choose which</t>
-  </si>
-  <si>
-    <t>Combine using</t>
-  </si>
-  <si>
-    <t>Strava if not form</t>
+    <t>Keep/preferred</t>
+  </si>
+  <si>
+    <t>Merger</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>y or x</t>
+  </si>
+  <si>
+    <t>x = strava, y = form. Merge if one is x and one is y</t>
+  </si>
+  <si>
+    <t>How to merge these 2 tables?</t>
+  </si>
+  <si>
+    <t>If date = date, type = type and one is x and one is y [elapsed time similar, name similar, time of day similar- not reliable] then rows combine to one</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -204,12 +224,42 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECD2FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -224,19 +274,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -244,6 +301,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFECD2FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -552,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4C340A-E411-844B-BA94-0985AA8EA7C9}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -581,212 +643,269 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4"/>
-      <c r="B3" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="3"/>
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="4"/>
-      <c r="B4" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="3"/>
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="4"/>
-      <c r="B5" t="s">
+      <c r="E5" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="4"/>
-      <c r="B6" t="s">
+      <c r="E6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="4"/>
-      <c r="B7" t="s">
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="4"/>
-      <c r="B8" t="s">
+      <c r="E8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="4"/>
-      <c r="B9" t="s">
+      <c r="E9" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="4"/>
-      <c r="B10" t="s">
+      <c r="E10" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="E11" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5"/>
-      <c r="B12" t="s">
+      <c r="E12" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="7"/>
+      <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="5"/>
-      <c r="B13" t="s">
+      <c r="E13" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="7"/>
+      <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="5"/>
-      <c r="B14" t="s">
+      <c r="E14" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="7"/>
+      <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="5"/>
-      <c r="B15" t="s">
+      <c r="E15" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="7"/>
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1" t="s">
+      <c r="E16" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" s="6"/>
+      <c r="E17" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="D22" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>